<commit_message>
90 Degree fix and event sorting
</commit_message>
<xml_diff>
--- a/Research/events.xlsx
+++ b/Research/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stijn Rogiest\Documents\GitHub\Beat-UltraDimension\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stijn Rogiest\Documents\GitHub\Beat-360fyer\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06EAD32-E3C5-49C5-86F3-940942F2CFB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5336E7A7-E64F-455E-80DB-679C54EA11A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="5430" windowWidth="21600" windowHeight="11385" xr2:uid="{EC74E5AC-0E7B-4503-B5AE-D193A85F8F2B}"/>
+    <workbookView xWindow="3240" yWindow="8625" windowWidth="21600" windowHeight="11385" xr2:uid="{EC74E5AC-0E7B-4503-B5AE-D193A85F8F2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Event type</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>bomb</t>
+  </si>
+  <si>
+    <t>rotate platform (90 mode)</t>
   </si>
 </sst>
 </file>
@@ -581,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA4622F-29DA-41BF-A069-173CDA174031}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,6 +721,17 @@
         <v>25</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>

</xml_diff>